<commit_message>
PCA and SVC added
</commit_message>
<xml_diff>
--- a/feature_importance.xlsx
+++ b/feature_importance.xlsx
@@ -445,7 +445,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.02473438984031321</v>
+        <v>0.02722538410199895</v>
       </c>
     </row>
     <row r="3">
@@ -455,7 +455,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.06480285679712322</v>
+        <v>0.06941825975158858</v>
       </c>
     </row>
     <row r="4">
@@ -465,7 +465,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.03232413872595431</v>
+        <v>0.03202480394679981</v>
       </c>
     </row>
     <row r="5">
@@ -475,7 +475,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.004127002214498431</v>
+        <v>0.004485720505407579</v>
       </c>
     </row>
     <row r="6">
@@ -485,7 +485,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.004232098599495134</v>
+        <v>0.003375344006408036</v>
       </c>
     </row>
     <row r="7">
@@ -495,7 +495,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.01116136209883817</v>
+        <v>0.01125127516263806</v>
       </c>
     </row>
     <row r="8">
@@ -505,7 +505,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.00712789421985091</v>
+        <v>0.007597872694945964</v>
       </c>
     </row>
     <row r="9">
@@ -515,7 +515,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.008181475485867987</v>
+        <v>0.009129540874050537</v>
       </c>
     </row>
     <row r="10">
@@ -525,7 +525,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.0009779779264749708</v>
+        <v>0.001074487404337631</v>
       </c>
     </row>
     <row r="11">
@@ -535,7 +535,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.1113133615118123</v>
+        <v>0.09129751316561714</v>
       </c>
     </row>
     <row r="12">
@@ -545,7 +545,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.01754527371634621</v>
+        <v>0.01455143107344255</v>
       </c>
     </row>
     <row r="13">
@@ -555,7 +555,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.0309400537381589</v>
+        <v>0.03113441218556192</v>
       </c>
     </row>
     <row r="14">
@@ -565,7 +565,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.01022061461327942</v>
+        <v>0.01012903924269608</v>
       </c>
     </row>
     <row r="15">
@@ -575,7 +575,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.001692905821536925</v>
+        <v>0.001323135676766408</v>
       </c>
     </row>
     <row r="16">
@@ -585,7 +585,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.002097752044317464</v>
+        <v>0.002262532587643698</v>
       </c>
     </row>
     <row r="17">
@@ -595,7 +595,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.2047216282349821</v>
+        <v>0.1943941231569433</v>
       </c>
     </row>
     <row r="18">
@@ -605,7 +605,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.2179676985410711</v>
+        <v>0.2299971750829252</v>
       </c>
     </row>
     <row r="19">
@@ -615,7 +615,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.1834706059901498</v>
+        <v>0.1994533815257453</v>
       </c>
     </row>
     <row r="20">
@@ -625,7 +625,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.001027566273679148</v>
+        <v>0.001251916978644955</v>
       </c>
     </row>
     <row r="21">
@@ -635,7 +635,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.0004161472750269772</v>
+        <v>0.0003543820996176175</v>
       </c>
     </row>
     <row r="22">
@@ -645,7 +645,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.0004464294371891248</v>
+        <v>0.0006884600586542392</v>
       </c>
     </row>
     <row r="23">
@@ -655,7 +655,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.02283630915037133</v>
+        <v>0.0206474243327993</v>
       </c>
     </row>
     <row r="24">
@@ -665,7 +665,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.01351532226952871</v>
+        <v>0.01333386200139725</v>
       </c>
     </row>
     <row r="25">
@@ -675,7 +675,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.0001395871495049155</v>
+        <v>5.211937984980118e-05</v>
       </c>
     </row>
     <row r="26">
@@ -685,7 +685,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.005753206335270818</v>
+        <v>0.005506532985097312</v>
       </c>
     </row>
     <row r="27">
@@ -695,7 +695,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.002361981236136054</v>
+        <v>0.002060336809977218</v>
       </c>
     </row>
     <row r="28">
@@ -705,7 +705,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>4.812433831054759e-05</v>
+        <v>5.395964464036869e-05</v>
       </c>
     </row>
     <row r="29">
@@ -715,7 +715,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.001190109825716702</v>
+        <v>0.001283925708030001</v>
       </c>
     </row>
     <row r="30">
@@ -725,7 +725,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.0003501395401397881</v>
+        <v>0.000384753721017454</v>
       </c>
     </row>
     <row r="31">
@@ -735,7 +735,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.006142669934124862</v>
+        <v>0.005920582190297914</v>
       </c>
     </row>
     <row r="32">
@@ -745,7 +745,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.001879774091810345</v>
+        <v>0.002010494057284897</v>
       </c>
     </row>
     <row r="33">
@@ -755,7 +755,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.006139049918438937</v>
+        <v>0.006210573606390271</v>
       </c>
     </row>
     <row r="34">
@@ -765,7 +765,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.0001144931046812289</v>
+        <v>0.000115244280784677</v>
       </c>
     </row>
   </sheetData>

</xml_diff>